<commit_message>
Now twilio launcher receives credentials and columns of interest as inputs
</commit_message>
<xml_diff>
--- a/input_example.xlsx
+++ b/input_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarlosBohm\requests_to_twilio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\requests_to_twilio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6428B2D-1044-4A1D-BDD2-C7D6353870E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA4760A-139F-4008-996B-6ED55A0A9FE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9EA10AB9-E7C1-4BAA-8028-5A12D0DF9A6D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{9EA10AB9-E7C1-4BAA-8028-5A12D0DF9A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Number</t>
   </si>
@@ -66,43 +66,37 @@
     <t>full_name</t>
   </si>
   <si>
-    <t>whatsapp:+5731111111111</t>
-  </si>
-  <si>
-    <t>whatsapp:+5731111111112</t>
-  </si>
-  <si>
-    <t>whatsapp:+5731111111113</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
     <t>Felipe</t>
   </si>
   <si>
-    <t>Kiara</t>
-  </si>
-  <si>
-    <t>Ana Examply</t>
-  </si>
-  <si>
-    <t>Felipe Ejemplares</t>
-  </si>
-  <si>
-    <t>Kiara Maria Raush</t>
-  </si>
-  <si>
     <t>enero</t>
   </si>
   <si>
-    <t>marzo</t>
-  </si>
-  <si>
     <t>working</t>
   </si>
   <si>
     <t>looking for a job</t>
+  </si>
+  <si>
+    <t>caseid</t>
+  </si>
+  <si>
+    <t>TestFelipe</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Carlos Bohm</t>
+  </si>
+  <si>
+    <t>whatsapp:+17733220947</t>
+  </si>
+  <si>
+    <t>whatsapp:+573206198169</t>
+  </si>
+  <si>
+    <t>Felipe Alamos</t>
   </si>
 </sst>
 </file>
@@ -455,18 +449,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EEC36A-96ED-4D29-A705-6FE23DFC514E}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,16 +488,19 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -515,21 +515,24 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
       </c>
       <c r="E3">
         <v>2020</v>
@@ -541,33 +544,10 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>2020</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>